<commit_message>
Enhance delivery and pickup summary pages with additional status totals and seller phone number, and improve delivery status update functionality
</commit_message>
<xml_diff>
--- a/adm/export/Data Pick Up.xlsx
+++ b/adm/export/Data Pick Up.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>DATA PICK UP</t>
   </si>
@@ -23,6 +23,9 @@
     <t>NO</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
     <t>KURIR PICK UP</t>
   </si>
   <si>
@@ -50,10 +53,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Tanggal</t>
-  </si>
-  <si>
-    <t>Kurir</t>
+    <t>Kurir Delivery</t>
   </si>
   <si>
     <t>Kode Resi</t>
@@ -71,7 +71,25 @@
     <t>Keterangan</t>
   </si>
   <si>
-    <t>22/07/2025</t>
+    <t>AMRI</t>
+  </si>
+  <si>
+    <t>WMGQ</t>
+  </si>
+  <si>
+    <t>DODI</t>
+  </si>
+  <si>
+    <t>CANCEL</t>
+  </si>
+  <si>
+    <t>SADAM</t>
+  </si>
+  <si>
+    <t>CKOR</t>
+  </si>
+  <si>
+    <t>UDIN</t>
   </si>
   <si>
     <t>ADMINISTRATOR</t>
@@ -81,9 +99,6 @@
   </si>
   <si>
     <t>ALEXA LEONARD</t>
-  </si>
-  <si>
-    <t>CANCEL</t>
   </si>
   <si>
     <t>TOTAL CANCEL:</t>
@@ -471,33 +486,34 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="2" max="2" width="6.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="17.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="20.281" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.855" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="21.566" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="15.139" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="20.281" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="12.568" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="16.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="11.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="13.854" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -522,18 +538,21 @@
       <c r="I4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -554,48 +573,103 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="B11" s="4">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="4">
+        <v>2194</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4">
+        <v>200</v>
+      </c>
+      <c r="H11" s="4">
+        <v>10</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="4">
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2192</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="4">
+        <v>90000</v>
+      </c>
+      <c r="H12" s="4">
+        <v>3000</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2172</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="4">
         <v>2000000</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H13" s="4">
         <v>23400</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="F12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2000000</v>
-      </c>
-      <c r="H12" s="2">
-        <v>23400</v>
+      <c r="I13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="F14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2090200</v>
+      </c>
+      <c r="H14" s="2">
+        <v>26410</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2063790</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update pickup status handling to reflect delivery status and improve query logic
</commit_message>
<xml_diff>
--- a/adm/export/Data Pick Up.xlsx
+++ b/adm/export/Data Pick Up.xlsx
@@ -92,7 +92,7 @@
     <t>UDIN</t>
   </si>
   <si>
-    <t>ADMINISTRATOR</t>
+    <t>ADEK</t>
   </si>
   <si>
     <t>9LB6</t>
@@ -590,10 +590,10 @@
         <v>20</v>
       </c>
       <c r="G11" s="4">
-        <v>200</v>
+        <v>22222</v>
       </c>
       <c r="H11" s="4">
-        <v>10</v>
+        <v>2222</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>21</v>
@@ -656,13 +656,13 @@
         <v>28</v>
       </c>
       <c r="G14" s="2">
-        <v>2090200</v>
+        <v>2112222</v>
       </c>
       <c r="H14" s="2">
-        <v>26410</v>
+        <v>28622</v>
       </c>
       <c r="I14" s="2">
-        <v>2063790</v>
+        <v>2083600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>